<commit_message>
Introduce ded settings, more unit tests
More unit tests
</commit_message>
<xml_diff>
--- a/cliprt/tests/test_preconfig_workbook.xlsx
+++ b/cliprt/tests/test_preconfig_workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhodges/VisualStudioCodeProjects/cliprt/cliprt/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB2568-7EB3-F240-A951-3DF17728A065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBBF696-81F8-C944-8FEF-95081E269C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="740" windowWidth="31940" windowHeight="18320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,18 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="179">
   <si>
     <t>Data Element</t>
-  </si>
-  <si>
-    <t>For Facebook targeting and API</t>
-  </si>
-  <si>
-    <t>For internal use (Searching and contacting)</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
   <si>
     <t>Dest WS</t>
@@ -62,9 +53,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Necessary</t>
-  </si>
-  <si>
     <t>birthday</t>
   </si>
   <si>
@@ -78,9 +66,6 @@
   </si>
   <si>
     <t>client name</t>
-  </si>
-  <si>
-    <t>will parse last word to last name and rest to first name</t>
   </si>
   <si>
     <t>first name</t>
@@ -98,16 +83,7 @@
     <t>phone</t>
   </si>
   <si>
-    <t>home phone will map to phone</t>
-  </si>
-  <si>
     <t>home phone</t>
-  </si>
-  <si>
-    <t>Necessary ("home," etc. not)</t>
-  </si>
-  <si>
-    <t>mapped</t>
   </si>
   <si>
     <t>mobile phone</t>
@@ -1077,225 +1053,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="16" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="B2"/>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="E2"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
+      <c r="B6"/>
+      <c r="D6" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="C9" t="s">
+        <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E6"/>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
+      <c r="C10" t="s">
+        <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
+      <c r="B11"/>
+      <c r="D11" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
+      <c r="D12" t="s">
+        <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="B14"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B16"/>
+      <c r="D16" t="s">
         <v>21</v>
-      </c>
-      <c r="E11"/>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14"/>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16"/>
-      <c r="G16" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1328,31 +1238,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1360,7 +1270,7 @@
         <v>100005800</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C2" s="3">
         <v>43882</v>
@@ -1369,19 +1279,19 @@
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1389,7 +1299,7 @@
         <v>100003575</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C3" s="3">
         <v>43564</v>
@@ -1399,19 +1309,19 @@
         <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1419,7 +1329,7 @@
         <v>100003465</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3">
         <v>43547</v>
@@ -1429,19 +1339,19 @@
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1449,7 +1359,7 @@
         <v>100005413</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3">
         <v>44022</v>
@@ -1459,19 +1369,19 @@
         <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1479,7 +1389,7 @@
         <v>100005723</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C6" s="3">
         <v>43871</v>
@@ -1489,19 +1399,19 @@
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1509,7 +1419,7 @@
         <v>100004341</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3">
         <v>43673</v>
@@ -1519,19 +1429,19 @@
         <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1539,7 +1449,7 @@
         <v>100006004</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C8" s="3">
         <v>43962</v>
@@ -1549,19 +1459,19 @@
         <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1569,7 +1479,7 @@
         <v>100003248</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C9" s="3">
         <v>43494</v>
@@ -1579,19 +1489,19 @@
         <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1599,7 +1509,7 @@
         <v>100005827</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C10" s="3">
         <v>43887</v>
@@ -1609,19 +1519,19 @@
         <v>45</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1629,7 +1539,7 @@
         <v>100005308</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C11" s="3">
         <v>43825</v>
@@ -1639,19 +1549,19 @@
         <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1659,25 +1569,25 @@
         <v>100005308</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3">
         <v>43825</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1685,7 +1595,7 @@
         <v>100004798</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C13" s="3">
         <v>43743</v>
@@ -1695,19 +1605,19 @@
         <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1715,7 +1625,7 @@
         <v>100001921</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C14" s="3">
         <v>42993</v>
@@ -1725,19 +1635,19 @@
         <v>57</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1745,7 +1655,7 @@
         <v>100005504</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C15" s="3">
         <v>43847</v>
@@ -1755,19 +1665,19 @@
         <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1775,7 +1685,7 @@
         <v>100002751</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C16" s="3">
         <v>43295</v>
@@ -1785,19 +1695,19 @@
         <v>63</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1805,7 +1715,7 @@
         <v>100002820</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C17" s="3">
         <v>43329</v>
@@ -1815,19 +1725,19 @@
         <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1835,7 +1745,7 @@
         <v>100003460</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C18" s="3">
         <v>43546</v>
@@ -1845,19 +1755,19 @@
         <v>69</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1865,7 +1775,7 @@
         <v>100005411</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C19" s="3">
         <v>43837</v>
@@ -1875,19 +1785,19 @@
         <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1895,7 +1805,7 @@
         <v>100004058</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C20" s="3">
         <v>43634</v>
@@ -1905,19 +1815,19 @@
         <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3086" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1955,342 +1865,342 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C2" s="11">
         <v>100005800</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C3" s="11">
         <v>100000058</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C4" s="11">
         <v>100005310</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11">
         <v>100003575</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C6" s="11">
         <v>100001587</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C7" s="11">
         <v>100001586</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C8" s="11">
         <v>100000536</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C9" s="11">
         <v>100003465</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C10" s="11">
         <v>100005413</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C11" s="11">
         <v>100000467</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C12" s="11">
         <v>100000468</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C13" s="11">
         <v>100001293</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C14" s="11">
         <v>100005723</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C15" s="11">
         <v>100004341</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C16" s="11">
         <v>100000414</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C17" s="11">
         <v>100002322</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C18" s="11">
         <v>100006004</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C19" s="11">
         <v>100003248</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C20" s="11">
         <v>100005827</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>